<commit_message>
FIX issue #159: Update `logistics.xslx`
</commit_message>
<xml_diff>
--- a/3.0.0/logistics.xlsx
+++ b/3.0.0/logistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UW31RY\work\papiNet-API\3.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684A313D-EBF3-45EC-8D0A-30B9EEAF3593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70830B-66FE-4CB9-B5AB-FD2507CA59DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="-21240" windowWidth="27270" windowHeight="20400" xr2:uid="{9275D04F-88B9-4E47-99DB-5102E40C57F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9275D04F-88B9-4E47-99DB-5102E40C57F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="72">
   <si>
     <t>ListOfSupplierOrders</t>
   </si>
@@ -248,17 +248,17 @@
     <t>sequenceCount</t>
   </si>
   <si>
-    <t>Issue #157</t>
-  </si>
-  <si>
-    <t>Issue #164</t>
+    <t>logisticsSupplierParty</t>
+  </si>
+  <si>
+    <t>logisticsDeliveryParty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,13 +298,23 @@
     </font>
     <font>
       <b/>
+      <strike/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +324,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -483,9 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
@@ -493,14 +494,26 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +544,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -578,13 +591,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -930,16 +943,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678FAC13-5025-4250-BD51-DD8155D9A76B}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.08984375" customWidth="1"/>
@@ -1165,59 +1178,67 @@
       <c r="B13" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>70</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B16" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1226,11 +1247,13 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
     </row>
@@ -1240,7 +1263,7 @@
       <c r="C19" s="8"/>
       <c r="D19" s="7"/>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1251,7 +1274,7 @@
       <c r="C20" s="8"/>
       <c r="D20" s="7"/>
       <c r="E20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -1262,80 +1285,68 @@
       <c r="C21" s="8"/>
       <c r="D21" s="7"/>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="46"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="43" t="s">
+      <c r="D24" s="30"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="47"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="44" t="s">
+      <c r="D25" s="45"/>
+      <c r="E25" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="25"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A26" s="25"/>
       <c r="B26" s="30"/>
       <c r="C26" s="25"/>
       <c r="D26" s="22"/>
       <c r="E26" s="30"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="3" t="s">
-        <v>6</v>
+      <c r="F26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" s="31" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1346,7 +1357,7 @@
       <c r="E27" s="30"/>
       <c r="F27" s="22"/>
       <c r="G27" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1356,8 +1367,8 @@
       <c r="D28" s="22"/>
       <c r="E28" s="30"/>
       <c r="F28" s="22"/>
-      <c r="G28" s="35" t="s">
-        <v>10</v>
+      <c r="G28" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1367,47 +1378,43 @@
       <c r="D29" s="22"/>
       <c r="E29" s="30"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="25"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="37" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="39" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="8"/>
-      <c r="D32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="4" t="s">
-        <v>21</v>
+      <c r="D32" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="39" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1415,12 +1422,12 @@
       <c r="B33" s="9"/>
       <c r="C33" s="8"/>
       <c r="D33" s="3" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1428,12 +1435,12 @@
       <c r="B34" s="9"/>
       <c r="C34" s="8"/>
       <c r="D34" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1441,12 +1448,12 @@
       <c r="B35" s="9"/>
       <c r="C35" s="8"/>
       <c r="D35" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1454,12 +1461,12 @@
       <c r="B36" s="9"/>
       <c r="C36" s="8"/>
       <c r="D36" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1467,12 +1474,12 @@
       <c r="B37" s="9"/>
       <c r="C37" s="8"/>
       <c r="D37" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1480,12 +1487,12 @@
       <c r="B38" s="9"/>
       <c r="C38" s="8"/>
       <c r="D38" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1493,12 +1500,12 @@
       <c r="B39" s="9"/>
       <c r="C39" s="8"/>
       <c r="D39" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1506,64 +1513,64 @@
       <c r="B40" s="9"/>
       <c r="C40" s="8"/>
       <c r="D40" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="8"/>
       <c r="B41" s="9"/>
       <c r="C41" s="8"/>
-      <c r="D41" s="4" t="s">
-        <v>30</v>
+      <c r="D41" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="5" t="s">
-        <v>30</v>
+      <c r="G41" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="8"/>
       <c r="B42" s="9"/>
       <c r="C42" s="8"/>
-      <c r="D42" s="4" t="s">
-        <v>51</v>
+      <c r="D42" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="5" t="s">
-        <v>51</v>
+      <c r="G42" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="8"/>
       <c r="B43" s="9"/>
       <c r="C43" s="8"/>
-      <c r="D43" s="5" t="s">
-        <v>31</v>
+      <c r="D43" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="6" t="s">
-        <v>31</v>
+      <c r="G43" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="5" t="s">
-        <v>32</v>
+      <c r="D44" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="6" t="s">
-        <v>32</v>
+      <c r="G44" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1571,12 +1578,12 @@
       <c r="B45" s="9"/>
       <c r="C45" s="8"/>
       <c r="D45" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1584,12 +1591,12 @@
       <c r="B46" s="9"/>
       <c r="C46" s="8"/>
       <c r="D46" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1597,130 +1604,128 @@
       <c r="B47" s="9"/>
       <c r="C47" s="8"/>
       <c r="D47" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49" s="8"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="14"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="18" t="s">
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" s="14"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="24" t="s">
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B51" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D51" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E51" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="32" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="7"/>
-      <c r="B50" s="3" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="7"/>
+      <c r="B52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="3" t="s">
+      <c r="C52" s="7"/>
+      <c r="D52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="33" t="s">
+      <c r="F52" s="7"/>
+      <c r="G52" s="33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" s="22"/>
-      <c r="B51" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="22"/>
-      <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="22"/>
-      <c r="B53" s="25"/>
+      <c r="B53" s="19" t="s">
+        <v>7</v>
+      </c>
       <c r="C53" s="22"/>
       <c r="D53" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>41</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E53" s="22"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="19" t="s">
-        <v>41</v>
-      </c>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A54" s="22"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="19" t="s">
-        <v>42</v>
-      </c>
+      <c r="A54" s="26"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="22"/>
       <c r="B55" s="25"/>
       <c r="C55" s="22"/>
       <c r="D55" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E55" s="22"/>
+        <v>41</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="F55" s="7"/>
       <c r="G55" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1728,12 +1733,14 @@
       <c r="B56" s="25"/>
       <c r="C56" s="22"/>
       <c r="D56" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E56" s="22"/>
+        <v>42</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="F56" s="7"/>
       <c r="G56" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -1741,33 +1748,33 @@
       <c r="B57" s="25"/>
       <c r="C57" s="22"/>
       <c r="D57" s="19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
+      <c r="G57" s="19" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="22"/>
-      <c r="B58" s="19" t="s">
-        <v>15</v>
-      </c>
+      <c r="B58" s="25"/>
       <c r="C58" s="22"/>
       <c r="D58" s="19" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="E58" s="22"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
+      <c r="G58" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="22"/>
-      <c r="B59" s="19" t="s">
-        <v>16</v>
-      </c>
+      <c r="B59" s="25"/>
       <c r="C59" s="22"/>
       <c r="D59" s="19" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E59" s="22"/>
       <c r="F59" s="7"/>
@@ -1776,137 +1783,141 @@
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="22"/>
       <c r="B60" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C60" s="22"/>
       <c r="D60" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="22"/>
+      <c r="B61" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="22"/>
+      <c r="D61" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="22"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="22"/>
+      <c r="B62" s="19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="11"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A62" s="23"/>
-      <c r="B62" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="23"/>
-      <c r="D62" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="22"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="20" t="s">
-        <v>18</v>
+      <c r="G62" s="19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="11"/>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="14"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="23"/>
+      <c r="B64" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="23"/>
+      <c r="D64" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="11"/>
+      <c r="B65" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="11"/>
-      <c r="D63" s="12" t="s">
+      <c r="C65" s="11"/>
+      <c r="D65" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="12" t="s">
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="12" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A64" s="7"/>
-      <c r="B64" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="7"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="7"/>
-      <c r="B66" s="8"/>
+      <c r="B66" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C66" s="7"/>
-      <c r="D66" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="G66" s="7"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" s="11"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="12" t="s">
-        <v>48</v>
+      <c r="A67" s="7"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="7"/>
-      <c r="B68" s="32" t="s">
-        <v>50</v>
-      </c>
+      <c r="B68" s="8"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="D68" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
+      <c r="G68" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" s="7"/>
-      <c r="B69" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="7"/>
-      <c r="B70" s="4" t="s">
-        <v>21</v>
+      <c r="B70" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -1917,7 +1928,7 @@
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="7"/>
       <c r="B71" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -1928,7 +1939,7 @@
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="7"/>
       <c r="B72" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -1939,7 +1950,7 @@
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
       <c r="B73" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -1950,7 +1961,7 @@
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="7"/>
       <c r="B74" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -1961,7 +1972,7 @@
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="7"/>
       <c r="B75" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -1972,7 +1983,7 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="7"/>
       <c r="B76" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
@@ -1983,7 +1994,7 @@
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="7"/>
       <c r="B77" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -1994,7 +2005,7 @@
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="7"/>
       <c r="B78" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -2004,8 +2015,8 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="7"/>
-      <c r="B79" s="5" t="s">
-        <v>30</v>
+      <c r="B79" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -2015,8 +2026,8 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="7"/>
-      <c r="B80" s="5" t="s">
-        <v>51</v>
+      <c r="B80" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -2026,8 +2037,8 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="7"/>
-      <c r="B81" s="6" t="s">
-        <v>31</v>
+      <c r="B81" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -2037,8 +2048,8 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="7"/>
-      <c r="B82" s="6" t="s">
-        <v>32</v>
+      <c r="B82" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -2049,7 +2060,7 @@
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="7"/>
       <c r="B83" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -2060,7 +2071,7 @@
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="7"/>
       <c r="B84" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -2071,7 +2082,7 @@
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="7"/>
       <c r="B85" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -2080,122 +2091,144 @@
       <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="11"/>
-      <c r="B86" s="24" t="s">
+      <c r="A86" s="7"/>
+      <c r="B86" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="7"/>
+      <c r="B87" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="11"/>
+      <c r="B88" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="11"/>
-      <c r="B87" s="12" t="s">
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="11"/>
+      <c r="B89" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="11"/>
-      <c r="D87" s="12" t="s">
+      <c r="C89" s="11"/>
+      <c r="D89" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E87" s="12" t="s">
+      <c r="E89" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F87" s="16"/>
-      <c r="G87" s="12" t="s">
+      <c r="F89" s="16"/>
+      <c r="G89" s="12" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="7"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F88" s="7"/>
-      <c r="G88" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="7"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E89" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F89" s="7"/>
-      <c r="G89" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="7"/>
-      <c r="B90" s="3"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>56</v>
+      <c r="D90" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F90" s="7"/>
-      <c r="G90" s="4" t="s">
-        <v>56</v>
+      <c r="G90" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="7"/>
-      <c r="B91" s="3"/>
+      <c r="B91" s="8"/>
       <c r="C91" s="7"/>
       <c r="D91" s="4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="7"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="7"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="11"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="21" t="s">
+      <c r="E93" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F93" s="7"/>
+      <c r="G93" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="11"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E92" s="21" t="s">
+      <c r="E94" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F92" s="11"/>
-      <c r="G92" s="21" t="s">
+      <c r="F94" s="11"/>
+      <c r="G94" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="17" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B93" s="16"/>
-      <c r="C93" s="17" t="s">
+      <c r="B95" s="16"/>
+      <c r="C95" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D93" s="16"/>
-      <c r="E93" s="16"/>
-      <c r="F93" s="29" t="s">
+      <c r="D95" s="16"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G93" s="16"/>
+      <c r="G95" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>